<commit_message>
paper tables and hyperparam tables
</commit_message>
<xml_diff>
--- a/results/BaggingClassifier_SVC.xlsx
+++ b/results/BaggingClassifier_SVC.xlsx
@@ -495,7 +495,7 @@
         <is>
           <t>Pipeline(steps=[('scaler', MinMaxScaler()),
                 ('selector',
-                 &lt;__main__.NamedFeatureSelector object at 0x7f1ee4580ee0&gt;),
+                 &lt;__main__.NamedFeatureSelector object at 0x7f1f9927ecd0&gt;),
                 ('model',
                  BaggingClassifier(estimator=SVC(C=1, kernel='linear',
                                                  random_state=42),
@@ -507,7 +507,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f1ef09867f0&gt;, 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__kernel': 'linear', 'model__estimator__class_weight': None, 'model__estimator__C': 1}</t>
+          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f1f9924c550&gt;, 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__kernel': 'linear', 'model__estimator__class_weight': None, 'model__estimator__C': 1}</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -644,7 +644,7 @@
         <is>
           <t>Pipeline(steps=[('scaler', MinMaxScaler()),
                 ('selector',
-                 &lt;__main__.NamedFeatureSelector object at 0x7f1ee4580c40&gt;),
+                 &lt;__main__.NamedFeatureSelector object at 0x7f1f9927e970&gt;),
                 ('model',
                  BaggingClassifier(estimator=SVC(C=1, kernel='linear',
                                                  random_state=42),
@@ -656,7 +656,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f1ef0975b80&gt;, 'scaler': MinMaxScaler(), 'model__n_estimators': 5, 'model__estimator__kernel': 'linear', 'model__estimator__class_weight': None, 'model__estimator__C': 1}</t>
+          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f1f992d7be0&gt;, 'scaler': MinMaxScaler(), 'model__n_estimators': 5, 'model__estimator__kernel': 'linear', 'model__estimator__class_weight': None, 'model__estimator__C': 1}</t>
         </is>
       </c>
       <c r="D5" t="n">

</xml_diff>